<commit_message>
Corrected BOM and eagle files before devices are manufactured
</commit_message>
<xml_diff>
--- a/Bill of Materials/electronicload-BOM-R3.00.xlsx
+++ b/Bill of Materials/electronicload-BOM-R3.00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Jasper\electronica\electronic load\R3\ElectronicLoadR3.00\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A340878-FA0E-4A2E-9147-6D8EAE2ABBA2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5CBB3202-DF9F-4D08-95C3-8FF9752C69A7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$23</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$25</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="100">
   <si>
     <t>Column1</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Hirose</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C3, C5, C7, C8 </t>
-  </si>
-  <si>
     <t>R3, R11</t>
   </si>
   <si>
@@ -319,6 +316,21 @@
   </si>
   <si>
     <t>AAVID THERMALLOY</t>
+  </si>
+  <si>
+    <t>100pF</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, C3, C8 </t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>C5</t>
   </si>
 </sst>
 </file>
@@ -943,10 +955,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="electronicload" displayName="electronicload" ref="A1:Q23" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:Q23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState ref="A2:Q23">
-    <sortCondition ref="B1:B23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="electronicload" displayName="electronicload" ref="A1:Q25" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:Q25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState ref="A2:Q25">
+    <sortCondition ref="B1:B25"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="18" name="Qty" queryTableFieldId="1"/>
@@ -1268,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,7 +1374,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>23</v>
@@ -1461,7 +1473,7 @@
         <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -1498,7 +1510,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>27</v>
@@ -1507,10 +1519,10 @@
         <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1529,7 +1541,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -1538,10 +1550,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1557,69 +1569,53 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1635,10 +1631,10 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
@@ -1647,7 +1643,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>23</v>
@@ -1685,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
@@ -1694,45 +1690,29 @@
         <v>18</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-      <c r="O10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -1741,43 +1721,60 @@
         <v>18</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
+      <c r="O11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>5</v>
+      <c r="A12" s="1">
+        <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="I12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1788,30 +1785,28 @@
         <v>35</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12">
-        <v>0.1</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="N12" s="1"/>
       <c r="O12" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>2</v>
+      <c r="A13" s="1">
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -1820,55 +1815,41 @@
         <v>18</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="G13" s="1"/>
-      <c r="I13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>97</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="G14" s="1"/>
       <c r="I14" s="1" t="s">
@@ -1881,16 +1862,19 @@
         <v>35</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="N14">
+        <v>0.1</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>35</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>35</v>
@@ -1898,10 +1882,10 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -1910,10 +1894,10 @@
         <v>18</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="G15" s="1"/>
       <c r="I15" s="1" t="s">
@@ -1946,37 +1930,32 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16">
-        <v>2480556</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="G16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>35</v>
@@ -1996,19 +1975,19 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" t="s">
-        <v>86</v>
-      </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" t="s">
-        <v>87</v>
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G17" s="1"/>
       <c r="I17" s="1" t="s">
@@ -2021,7 +2000,7 @@
         <v>35</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>35</v>
@@ -2041,28 +2020,31 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
+      </c>
+      <c r="H18">
+        <v>2480556</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>35</v>
@@ -2088,23 +2070,21 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="1"/>
       <c r="I19" s="1" t="s">
         <v>35</v>
       </c>
@@ -2135,135 +2115,229 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="G22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" t="s">
         <v>90</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E21" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="E24" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>1</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23">
+      <c r="G25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25">
         <v>2554981</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K23" s="1" t="s">
+      <c r="J25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O23" s="1" t="s">
+      <c r="L25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q23" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q25" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>